<commit_message>
Cosmetic changes: VAT source file
Deleted comments
</commit_message>
<xml_diff>
--- a/source_data/oecd_vat_gst_rates_ctt_trends.xlsx
+++ b/source_data/oecd_vat_gst_rates_ctt_trends.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexanderMengden\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F48C8-5FDF-4C4E-900F-C67C760B66D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CD44B2-8A28-4DE1-969D-148181012E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,36 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={8295ACC6-A58B-48F1-A5C6-E29DBD2CCBAD}</author>
-    <author>tc={608F8682-E7EB-4EAE-9183-615807906989}</author>
-  </authors>
-  <commentList>
-    <comment ref="V12" authorId="0" shapeId="0" xr:uid="{8295ACC6-A58B-48F1-A5C6-E29DBD2CCBAD}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ab 2025 - deshalb Abweichung zu OECD 2024</t>
-      </text>
-    </comment>
-    <comment ref="V33" authorId="1" shapeId="0" xr:uid="{608F8682-E7EB-4EAE-9183-615807906989}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ab 2025 - deshalb Abweichung zu OECD 2024
-</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>Australia</t>
   </si>
@@ -274,57 +246,9 @@
     <t xml:space="preserve"> - </t>
   </si>
   <si>
-    <t>PWC</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Standard 22%, Reduced rates 0%, 5%, 9%</t>
-  </si>
-  <si>
-    <t>Reduced rates 18%, 5%, 0%</t>
-  </si>
-  <si>
-    <t>Reduced rates 0%, 9%, 13,5%</t>
-  </si>
-  <si>
-    <t>Standard (2025) 18%</t>
-  </si>
-  <si>
-    <t>Standard 17%</t>
-  </si>
-  <si>
-    <t>Regional rates 22%, 16% &amp; 12%, 9%, 4%</t>
-  </si>
-  <si>
-    <t>Standard (2025) 23% Reduced Rates (2025) 19%, 5%</t>
-  </si>
-  <si>
-    <t>Standard 25.5%, Reduced rates 10%, 14%, 0%</t>
-  </si>
-  <si>
-    <t>reduced rates 13, 6, 4</t>
-  </si>
-  <si>
-    <t>Standard 8,1% Reduced rate 0, 2,6%, 3,8%</t>
-  </si>
-  <si>
-    <t>Reduced rates 0, 12%</t>
-  </si>
-  <si>
-    <t>(2025) Reduced rates 15, 12, 11.11, 0</t>
-  </si>
-  <si>
-    <t>reduced rates 1, 2, 4, 0.5</t>
-  </si>
-  <si>
     <t>0/12.0</t>
   </si>
   <si>
-    <t>(2024) Standard 22%, (2025) Standard 24%, Reduced rates 0%, 13%, 9% (2025)</t>
-  </si>
-  <si>
     <t>0.0/9.0/13.0</t>
   </si>
   <si>
@@ -340,9 +264,6 @@
     <t>0.0/2.6/3.8</t>
   </si>
   <si>
-    <t>Bloomberg</t>
-  </si>
-  <si>
     <t>0/4.0/10.0</t>
   </si>
   <si>
@@ -355,16 +276,7 @@
     <t>0/1.0/2.0/4.0</t>
   </si>
   <si>
-    <t>(31.08.2024) Standard 25.5%, Reduced rates 10%, 14%, 0%</t>
-  </si>
-  <si>
     <t>5.0/12.0</t>
-  </si>
-  <si>
-    <t>Reduced rates  5%, 12%</t>
-  </si>
-  <si>
-    <t>Reduced rates 5%, 12%</t>
   </si>
   <si>
     <t>0.0/12.0/15.0</t>
@@ -764,7 +676,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -811,31 +723,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,12 +752,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,7 +861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1022,22 +911,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1046,8 +932,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,9 +953,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Andrea Nieder" id="{B994DDF8-FD50-4569-8CB1-C2947F69F28C}" userId="eeed051e0af845b7" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,24 +1217,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="V12" dT="2025-05-21T10:35:24.17" personId="{B994DDF8-FD50-4569-8CB1-C2947F69F28C}" id="{8295ACC6-A58B-48F1-A5C6-E29DBD2CCBAD}">
-    <text>Ab 2025 - deshalb Abweichung zu OECD 2024</text>
-  </threadedComment>
-  <threadedComment ref="V33" dT="2025-05-21T10:35:40.79" personId="{B994DDF8-FD50-4569-8CB1-C2947F69F28C}" id="{608F8682-E7EB-4EAE-9183-615807906989}">
-    <text xml:space="preserve">Ab 2025 - deshalb Abweichung zu OECD 2024
-</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1361,37 +1233,36 @@
     <col min="19" max="21" width="4.86328125" customWidth="1"/>
     <col min="22" max="22" width="10.86328125" customWidth="1"/>
     <col min="23" max="23" width="15.3984375" customWidth="1"/>
-    <col min="24" max="24" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:23" ht="14.65" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-    </row>
-    <row r="2" spans="1:25" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="12">
         <v>2005</v>
       </c>
@@ -1458,14 +1329,8 @@
       <c r="W2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="X2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1535,14 +1400,8 @@
       <c r="W3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1612,14 +1471,8 @@
       <c r="W4" s="14">
         <v>19</v>
       </c>
-      <c r="X4" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
@@ -1689,14 +1542,8 @@
       <c r="W5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1766,14 +1613,8 @@
       <c r="W6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="X6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1843,14 +1684,8 @@
       <c r="W7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -1920,14 +1755,8 @@
       <c r="W8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X8" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -1980,17 +1809,11 @@
         <v>13</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="W9" s="15"/>
-      <c r="X9" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y9" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -2055,19 +1878,13 @@
         <v>21</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="W10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X10" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
@@ -2137,14 +1954,8 @@
       <c r="W11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -2208,20 +2019,14 @@
       <c r="U12" s="10">
         <v>24</v>
       </c>
-      <c r="V12" s="21" t="s">
-        <v>80</v>
+      <c r="V12" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="W12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X12" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y12" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>55</v>
       </c>
@@ -2291,14 +2096,8 @@
       <c r="W13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="22.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:23" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -2368,14 +2167,8 @@
       <c r="W14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="X14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -2445,14 +2238,8 @@
       <c r="W15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X15" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -2517,19 +2304,13 @@
         <v>24</v>
       </c>
       <c r="V16" s="14" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="W16" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="X16" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y16" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
@@ -2594,19 +2375,13 @@
         <v>27</v>
       </c>
       <c r="V17" s="15" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="W17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X17" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2676,14 +2451,8 @@
       <c r="W18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X18" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -2753,14 +2522,8 @@
       <c r="W19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y19" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -2830,14 +2593,8 @@
       <c r="W20" s="14">
         <v>0</v>
       </c>
-      <c r="X20" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
@@ -2907,14 +2664,8 @@
       <c r="W21" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X21" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -2984,14 +2735,8 @@
       <c r="W22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -3061,14 +2806,8 @@
       <c r="W23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X23" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -3133,19 +2872,13 @@
         <v>21</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="W24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X24" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -3215,14 +2948,8 @@
       <c r="W25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X25" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -3292,14 +3019,8 @@
       <c r="W26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X26" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -3369,14 +3090,8 @@
       <c r="W27" s="15">
         <v>8</v>
       </c>
-      <c r="X27" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -3446,14 +3161,8 @@
       <c r="W28" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X28" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -3523,14 +3232,8 @@
       <c r="W29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X29" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -3595,19 +3298,13 @@
         <v>25</v>
       </c>
       <c r="V30" s="10" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="W30" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X30" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y30" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -3677,14 +3374,8 @@
       <c r="W31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X31" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -3752,16 +3443,10 @@
         <v>18</v>
       </c>
       <c r="W32" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="X32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -3825,20 +3510,14 @@
       <c r="U33" s="11">
         <v>23</v>
       </c>
-      <c r="V33" s="21" t="s">
-        <v>83</v>
+      <c r="V33" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="W33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X33" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
@@ -3908,14 +3587,8 @@
       <c r="W34" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X34" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
@@ -3980,19 +3653,13 @@
         <v>21</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="W35" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="X35" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y35" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -4062,14 +3729,8 @@
       <c r="W36" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>60</v>
       </c>
@@ -4134,19 +3795,13 @@
         <v>8.1</v>
       </c>
       <c r="V37" s="15" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="W37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
@@ -4216,14 +3871,8 @@
       <c r="W38" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X38" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
@@ -4293,14 +3942,8 @@
       <c r="W39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X39" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>7</v>
       </c>
@@ -4380,586 +4023,577 @@
       <c r="V40" s="8"/>
       <c r="W40" s="17"/>
     </row>
-    <row r="41" spans="1:25" ht="17.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
-      <c r="P41" s="28"/>
-      <c r="Q41" s="28"/>
+    <row r="41" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A42" s="25" t="s">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A42" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="26"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
-      <c r="Q42" s="26"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A43" s="26" t="s">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A43" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-    </row>
-    <row r="45" spans="1:25" ht="53.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="23"/>
-    </row>
-    <row r="46" spans="1:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23"/>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="23"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="23"/>
-    </row>
-    <row r="47" spans="1:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="23"/>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="23"/>
-      <c r="S47" s="23"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="23"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A48" s="26" t="s">
+    <row r="44" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+    </row>
+    <row r="45" spans="1:23" ht="53.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+    </row>
+    <row r="46" spans="1:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+    </row>
+    <row r="47" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A48" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="26"/>
+      <c r="B48" s="20"/>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
-      <c r="P49" s="23"/>
-      <c r="Q49" s="23"/>
-      <c r="R49" s="23"/>
-      <c r="S49" s="23"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="23"/>
-      <c r="V49" s="23"/>
-      <c r="W49" s="23"/>
+      <c r="A49" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="19"/>
+      <c r="T49" s="19"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19"/>
     </row>
     <row r="50" spans="1:23" ht="68.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="23"/>
-      <c r="Q50" s="23"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="23"/>
-      <c r="V50" s="23"/>
-      <c r="W50" s="23"/>
+      <c r="A50" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
     </row>
     <row r="51" spans="1:23" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="23"/>
-      <c r="M51" s="23"/>
-      <c r="N51" s="23"/>
-      <c r="O51" s="23"/>
-      <c r="P51" s="23"/>
-      <c r="Q51" s="23"/>
-      <c r="R51" s="23"/>
-      <c r="S51" s="23"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="23"/>
-      <c r="V51" s="23"/>
-      <c r="W51" s="23"/>
+      <c r="A51" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="19"/>
+      <c r="T51" s="19"/>
+      <c r="U51" s="19"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="19"/>
     </row>
     <row r="52" spans="1:23" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="23"/>
-      <c r="M52" s="23"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="23"/>
-      <c r="P52" s="23"/>
-      <c r="Q52" s="23"/>
-      <c r="R52" s="23"/>
-      <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="23"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="23"/>
+      <c r="A52" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
+      <c r="U52" s="19"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="19"/>
     </row>
     <row r="53" spans="1:23" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="23"/>
-      <c r="M53" s="23"/>
-      <c r="N53" s="23"/>
-      <c r="O53" s="23"/>
-      <c r="P53" s="23"/>
-      <c r="Q53" s="23"/>
-      <c r="R53" s="23"/>
-      <c r="S53" s="23"/>
-      <c r="T53" s="23"/>
-      <c r="U53" s="23"/>
-      <c r="V53" s="23"/>
-      <c r="W53" s="23"/>
+      <c r="A53" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="19"/>
+      <c r="T53" s="19"/>
+      <c r="U53" s="19"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
     </row>
     <row r="54" spans="1:23" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="23"/>
-      <c r="M54" s="23"/>
-      <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
-      <c r="P54" s="23"/>
-      <c r="Q54" s="23"/>
-      <c r="R54" s="23"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="23"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="23"/>
+      <c r="A54" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="19"/>
+      <c r="T54" s="19"/>
+      <c r="U54" s="19"/>
+      <c r="V54" s="19"/>
+      <c r="W54" s="19"/>
     </row>
     <row r="55" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
-      <c r="N55" s="26"/>
-      <c r="O55" s="26"/>
-      <c r="P55" s="26"/>
-      <c r="Q55" s="26"/>
-      <c r="R55" s="26"/>
-      <c r="S55" s="26"/>
-      <c r="T55" s="26"/>
-      <c r="U55" s="26"/>
-      <c r="V55" s="26"/>
-      <c r="W55" s="26"/>
+      <c r="A55" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="20"/>
+      <c r="V55" s="20"/>
+      <c r="W55" s="20"/>
     </row>
     <row r="56" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="23"/>
-      <c r="N56" s="23"/>
-      <c r="O56" s="23"/>
-      <c r="P56" s="23"/>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="23"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="23"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="23"/>
+      <c r="A56" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="19"/>
+      <c r="R56" s="19"/>
+      <c r="S56" s="19"/>
+      <c r="T56" s="19"/>
+      <c r="U56" s="19"/>
+      <c r="V56" s="19"/>
+      <c r="W56" s="19"/>
     </row>
     <row r="57" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="M57" s="23"/>
-      <c r="N57" s="23"/>
-      <c r="O57" s="23"/>
-      <c r="P57" s="23"/>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="23"/>
-      <c r="S57" s="23"/>
-      <c r="T57" s="23"/>
-      <c r="U57" s="23"/>
-      <c r="V57" s="23"/>
-      <c r="W57" s="23"/>
+      <c r="A57" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="19"/>
+      <c r="S57" s="19"/>
+      <c r="T57" s="19"/>
+      <c r="U57" s="19"/>
+      <c r="V57" s="19"/>
+      <c r="W57" s="19"/>
     </row>
     <row r="58" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="29"/>
-      <c r="O58" s="29"/>
-      <c r="P58" s="29"/>
-      <c r="Q58" s="29"/>
-      <c r="R58" s="29"/>
-      <c r="S58" s="29"/>
-      <c r="T58" s="29"/>
-      <c r="U58" s="29"/>
-      <c r="V58" s="29"/>
-      <c r="W58" s="29"/>
+      <c r="A58" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="21"/>
+      <c r="R58" s="21"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="21"/>
+      <c r="U58" s="21"/>
+      <c r="V58" s="21"/>
+      <c r="W58" s="21"/>
     </row>
     <row r="59" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="23"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="23"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="23"/>
+      <c r="A59" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
+      <c r="P59" s="19"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="19"/>
+      <c r="S59" s="19"/>
+      <c r="T59" s="19"/>
+      <c r="U59" s="19"/>
+      <c r="V59" s="19"/>
+      <c r="W59" s="19"/>
     </row>
     <row r="60" spans="1:23" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
-      <c r="P60" s="23"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="23"/>
-      <c r="S60" s="23"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="23"/>
-      <c r="V60" s="23"/>
-      <c r="W60" s="23"/>
+      <c r="A60" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
+      <c r="N60" s="19"/>
+      <c r="O60" s="19"/>
+      <c r="P60" s="19"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="19"/>
+      <c r="S60" s="19"/>
+      <c r="T60" s="19"/>
+      <c r="U60" s="19"/>
+      <c r="V60" s="19"/>
+      <c r="W60" s="19"/>
     </row>
     <row r="61" spans="1:23" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23"/>
-      <c r="I61" s="23"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="23"/>
-      <c r="M61" s="23"/>
-      <c r="N61" s="23"/>
-      <c r="O61" s="23"/>
-      <c r="P61" s="23"/>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="23"/>
-      <c r="S61" s="23"/>
-      <c r="T61" s="23"/>
-      <c r="U61" s="23"/>
-      <c r="V61" s="23"/>
-      <c r="W61" s="23"/>
+      <c r="A61" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
+      <c r="P61" s="19"/>
+      <c r="Q61" s="19"/>
+      <c r="R61" s="19"/>
+      <c r="S61" s="19"/>
+      <c r="T61" s="19"/>
+      <c r="U61" s="19"/>
+      <c r="V61" s="19"/>
+      <c r="W61" s="19"/>
     </row>
     <row r="62" spans="1:23" ht="86.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="23"/>
-      <c r="I62" s="23"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="23"/>
-      <c r="N62" s="23"/>
-      <c r="O62" s="23"/>
-      <c r="P62" s="23"/>
-      <c r="Q62" s="23"/>
-      <c r="R62" s="23"/>
-      <c r="S62" s="23"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="23"/>
-      <c r="V62" s="23"/>
-      <c r="W62" s="23"/>
+      <c r="A62" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="19"/>
+      <c r="P62" s="19"/>
+      <c r="Q62" s="19"/>
+      <c r="R62" s="19"/>
+      <c r="S62" s="19"/>
+      <c r="T62" s="19"/>
+      <c r="U62" s="19"/>
+      <c r="V62" s="19"/>
+      <c r="W62" s="19"/>
     </row>
     <row r="64" spans="1:23" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A62:W62"/>
-    <mergeCell ref="A60:W60"/>
-    <mergeCell ref="A61:W61"/>
-    <mergeCell ref="A54:W54"/>
-    <mergeCell ref="A56:W56"/>
-    <mergeCell ref="A57:W57"/>
-    <mergeCell ref="A59:W59"/>
-    <mergeCell ref="A55:W55"/>
-    <mergeCell ref="A58:W58"/>
     <mergeCell ref="A53:W53"/>
     <mergeCell ref="A49:W49"/>
     <mergeCell ref="A52:W52"/>
@@ -4974,9 +4608,17 @@
     <mergeCell ref="A47:W47"/>
     <mergeCell ref="A50:W50"/>
     <mergeCell ref="A51:W51"/>
+    <mergeCell ref="A62:W62"/>
+    <mergeCell ref="A60:W60"/>
+    <mergeCell ref="A61:W61"/>
+    <mergeCell ref="A54:W54"/>
+    <mergeCell ref="A56:W56"/>
+    <mergeCell ref="A57:W57"/>
+    <mergeCell ref="A59:W59"/>
+    <mergeCell ref="A55:W55"/>
+    <mergeCell ref="A58:W58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>